<commit_message>
cambios de las vistas
</commit_message>
<xml_diff>
--- a/document/progresivos-semanal.xlsx
+++ b/document/progresivos-semanal.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\CASINOMARCOPOLO\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650997A7-8755-44FD-9A6F-A3D31DCEE3CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B0F3A7-2294-4F70-B209-DEE1CD08F8A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{21EF4714-7C9B-4AA5-B12B-FFC53C53842E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{21EF4714-7C9B-4AA5-B12B-FFC53C53842E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$E$23</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -645,10 +645,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8D934C-B6E8-4251-B65A-4EFF1D7806E4}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +671,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -687,7 +688,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -704,7 +705,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -738,7 +739,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -755,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -772,7 +773,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -790,7 +791,7 @@
       </c>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -807,7 +808,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -824,7 +825,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -841,7 +842,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -858,7 +859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -875,7 +876,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -892,7 +893,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>38</v>
       </c>
@@ -909,7 +910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -943,7 +944,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -960,7 +961,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1011,7 +1012,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1028,7 +1029,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1046,7 +1047,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{0BE739B4-335E-45AD-A050-B99D25CEDCC3}"/>
+  <autoFilter ref="A1:E23" xr:uid="{0BE739B4-335E-45AD-A050-B99D25CEDCC3}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="MP100"/>
+        <filter val="MP108"/>
+        <filter val="MP15"/>
+        <filter val="MP53"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1056,7 +1066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2974C24-6C63-4F9B-85C7-371F02AB740D}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>